<commit_message>
cambios director y participante
</commit_message>
<xml_diff>
--- a/public/Plantillas/1.3-Número-Horas-Docentes.xlsx
+++ b/public/Plantillas/1.3-Número-Horas-Docentes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ESPE_2023\sistema_vinculacion\sistema_vinculacion\public\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\OneDrive\Escritorio\TesisVersionBeta\Tesis_Final_Version\public\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{553FB3C6-5C3B-4C7B-A74C-12166216066F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE27CD16-6A2A-482A-BACE-D1097DAE0097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="540" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="43" r:id="rId1"/>
@@ -24,8 +24,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -138,7 +136,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -239,26 +237,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="hair">
-        <color indexed="64"/>
-      </top>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -284,9 +267,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -311,7 +291,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -337,9 +317,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -364,13 +341,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>244477</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>225426</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2447103</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>225429</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -419,13 +396,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>372534</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>209549</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>541868</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>16934</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -545,13 +522,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>916940</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>1047754</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -600,13 +577,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>135465</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>211666</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>677333</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>16933</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -727,13 +704,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>423333</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>33866</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>262467</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>33867</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1068,10 +1045,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="18" x14ac:dyDescent="0.3"/>
@@ -1090,32 +1067,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
     </row>
     <row r="2" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
     </row>
@@ -1124,14 +1101,14 @@
       <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
     </row>
     <row r="4" spans="1:12" ht="6.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
@@ -1146,26 +1123,26 @@
       <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:12" s="6" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="22"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="21"/>
     </row>
     <row r="6" spans="1:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="26"/>
-      <c r="B6" s="24"/>
+      <c r="A6" s="25"/>
+      <c r="B6" s="23"/>
       <c r="C6" s="7" t="s">
         <v>2</v>
       </c>
@@ -1192,94 +1169,80 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="17">
+      <c r="A7" s="16">
         <v>1</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="27"/>
-    </row>
-    <row r="8" spans="1:12" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="18"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-    </row>
-    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="10"/>
-      <c r="B9" s="11" t="s">
+      <c r="B7" s="16"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="17"/>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="9"/>
+      <c r="B8" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="12">
-        <f>SUM(J6:J8)</f>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="11">
+        <f>SUM(J6:J7)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
+      <c r="B13" s="14"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
-      <c r="B14" s="15"/>
+      <c r="B14" s="12"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B15" s="13"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B16" s="6"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B18" s="1" t="s">
+      <c r="B15" s="6"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17" s="1" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="A7:A8"/>
+  <mergeCells count="6">
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="C5:J5"/>

</xml_diff>

<commit_message>
arreglo docente participante docu,entacion
</commit_message>
<xml_diff>
--- a/public/Plantillas/1.3-Número-Horas-Docentes.xlsx
+++ b/public/Plantillas/1.3-Número-Horas-Docentes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tesis\Tesis_Final_Version\Tesis_Final_Version\public\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\OneDrive\Escritorio\TesisVersionBeta\Tesis_Final_Version\public\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4833A54-07A7-4784-BD9F-8110D3E2253F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{739CBB21-03A3-4F9E-A3D5-9B27C58A5863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="540" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="43" r:id="rId1"/>
@@ -745,9 +745,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -785,9 +785,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -820,26 +820,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -872,26 +855,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1068,25 +1034,25 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:J2"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="18" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="38.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="36.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="30.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="26.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" style="6" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="3.6640625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="38.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="36.44140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="30.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="26.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="20.109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="17.44140625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="15.44140625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" style="6" customWidth="1"/>
+    <col min="11" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>3</v>
       </c>
@@ -1100,7 +1066,7 @@
       <c r="I1" s="18"/>
       <c r="J1" s="18"/>
     </row>
-    <row r="2" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>9</v>
       </c>
@@ -1116,7 +1082,7 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="4" t="s">
         <v>4</v>
@@ -1130,7 +1096,7 @@
       <c r="I3" s="18"/>
       <c r="J3" s="18"/>
     </row>
-    <row r="4" spans="1:12" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="6.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
@@ -1142,7 +1108,7 @@
       <c r="I4" s="5"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:12" s="6" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" s="6" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="24" t="s">
         <v>1</v>
       </c>
@@ -1160,7 +1126,7 @@
       <c r="I5" s="20"/>
       <c r="J5" s="21"/>
     </row>
-    <row r="6" spans="1:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="25"/>
       <c r="B6" s="23"/>
       <c r="C6" s="7" t="s">
@@ -1188,7 +1154,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="49.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16">
         <v>1</v>
       </c>
@@ -1202,7 +1168,7 @@
       <c r="I7" s="15"/>
       <c r="J7" s="17"/>
     </row>
-    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9"/>
       <c r="B8" s="10" t="s">
         <v>0</v>
@@ -1219,11 +1185,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="12"/>
       <c r="C11" s="13"/>
@@ -1235,7 +1201,7 @@
       <c r="I11" s="13"/>
       <c r="J11" s="13"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="14"/>
       <c r="C12" s="6"/>
@@ -1246,17 +1212,20 @@
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="14"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B14" s="12"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B15" s="6"/>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>15</v>
       </c>

</xml_diff>